<commit_message>
Trying to use hw pwm timers
</commit_message>
<xml_diff>
--- a/pinout.xlsx
+++ b/pinout.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\School\Semester_8\Real-time\workspace\Roomba\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{682632C1-B8AB-4716-B0D8-4BF409D0869B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{112901CC-3D0C-4113-9168-BEA5CE567E08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="180" windowWidth="25440" windowHeight="15390" xr2:uid="{1CBDC2BD-5AC2-4ABF-9328-2652AF8BD22D}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{1CBDC2BD-5AC2-4ABF-9328-2652AF8BD22D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="60">
   <si>
     <t>FUNCTION</t>
   </si>
@@ -179,6 +179,42 @@
   </si>
   <si>
     <t>https://lastminuteengineers.com/l298n-dc-stepper-driver-arduino-tutorial/</t>
+  </si>
+  <si>
+    <t>5-35V</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>top on sides is for power out</t>
+  </si>
+  <si>
+    <t>bottom on sides is for gnd out</t>
+  </si>
+  <si>
+    <t>lidar not dependent</t>
+  </si>
+  <si>
+    <t>motor dependent on lidar</t>
+  </si>
+  <si>
+    <t>metric depeent on motor</t>
+  </si>
+  <si>
+    <t>screen dependent on metric</t>
+  </si>
+  <si>
+    <t>tick count for each task</t>
+  </si>
+  <si>
+    <t>lidar 51</t>
+  </si>
+  <si>
+    <t>display 120</t>
+  </si>
+  <si>
+    <t>motor could be main thread</t>
   </si>
 </sst>
 </file>
@@ -231,6 +267,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1171064</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>142490</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E56853B6-8784-87C7-CC8F-9A147674B248}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3886200" y="3924300"/>
+          <a:ext cx="4085714" cy="3076190"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -530,10 +615,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{165A6F1F-33DE-4A18-BB5B-97FB7317C654}">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -545,7 +630,7 @@
     <col min="10" max="10" width="94.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -568,7 +653,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -591,7 +676,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -614,7 +699,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -631,7 +716,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -654,7 +739,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -671,7 +756,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -688,7 +773,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -705,7 +790,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -728,7 +813,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -745,7 +830,18 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11" t="s">
+        <v>48</v>
+      </c>
+      <c r="K11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -761,8 +857,106 @@
       <c r="E12" t="s">
         <v>34</v>
       </c>
+      <c r="I12">
+        <v>2</v>
+      </c>
+      <c r="J12" t="s">
+        <v>44</v>
+      </c>
+      <c r="K12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I13">
+        <v>3</v>
+      </c>
+      <c r="J13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I14">
+        <v>4</v>
+      </c>
+      <c r="J14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>52</v>
+      </c>
+      <c r="I15">
+        <v>5</v>
+      </c>
+      <c r="J15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>53</v>
+      </c>
+      <c r="I16">
+        <v>6</v>
+      </c>
+      <c r="J16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>54</v>
+      </c>
+      <c r="I17">
+        <v>7</v>
+      </c>
+      <c r="J17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>55</v>
+      </c>
+      <c r="I18">
+        <v>8</v>
+      </c>
+      <c r="J18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I19">
+        <v>9</v>
+      </c>
+      <c r="J19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="24" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="26" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>59</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>